<commit_message>
game loop files have been started
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4716032-C37A-4197-8EC7-1BE0BE26D7DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97735A4D-8BA8-4A3D-8A16-A5479B99EB52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31110" yWindow="540" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -155,6 +155,9 @@
   <si>
     <t>Really just trying to figure out what I need to add to get this to convert to C! 
 Can't get Unity working no matter how many versions I uninstall and reinstall so that's great… Why can't I get a single version working?!?</t>
+  </si>
+  <si>
+    <t>Working on the game loop files - trying to figure out how this is going to work - what needs to return bools, what returns ints, what needs a more complicated function in the game loop file with additional game logic…</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>16.750000000000007</c:v>
+                  <c:v>25.249999999999918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -381,7 +384,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>163.25</c:v>
+                  <c:v>154.75000000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1445,7 +1448,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1472,7 @@
       </c>
       <c r="E1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>16.750000000000007</v>
+        <v>25.249999999999918</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1478,14 +1481,14 @@
       </c>
       <c r="B2" s="9">
         <f ca="1">B1-TODAY()</f>
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="10">
         <f>180-_xlfn.NUMBERVALUE(E1)</f>
-        <v>163.25</v>
+        <v>154.75000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1502,7 +1505,7 @@
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,21 +1730,29 @@
       </c>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12" s="1">
         <v>43629</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E12" s="5">
+        <v>90</v>
+      </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="11"/>
+        <v>0.35416666666666663</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2533,7 +2544,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>0.69791666666666652</v>
+        <v>1.052083333333333</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2682,7 +2693,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Successfully calling a function in submarine.adb and returning updated sub value
Although it's giving an unexpected and incorrect value...
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48E13A2-074D-4C90-B237-359503363087}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B49CCF-A637-4A05-B5AA-94D1FDA53CC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33990" yWindow="570" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
@@ -160,7 +160,8 @@
     <t>Working on the game loop files - trying to figure out how this is going to work - what needs to return bools, what returns ints, what needs a more complicated function in the game loop file with additional game logic…</t>
   </si>
   <si>
-    <t>More work on the game loop files - working on a function to return the sub stats that can be called every frame to keep the UI up to date and to test the emergency surface code in the submarine files</t>
+    <t>More work on the game loop files - created a function to return the sub stats that I can call after any user action. Created a temp function to seal all the doors so I can test the movement before anything else. Successfully managing to alter the depth and return a different value but it's not the values I'm expecting - think there's a problem with data type conversion when converting into C. 
+Overall, there's a skeleton game loop created in SPARK which is allowing me to access and manipulate the sub pos and movements from Unity which seems like a decent proof of concept but there are still some bugs to work out.</t>
   </si>
 </sst>
 </file>
@@ -345,7 +346,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>32.749999999999915</c:v>
+                  <c:v>31.750000000000082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,7 +388,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>147.25000000000011</c:v>
+                  <c:v>148.24999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,7 +1476,7 @@
       </c>
       <c r="E1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>32.749999999999915</v>
+        <v>31.750000000000082</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1491,7 +1492,7 @@
       </c>
       <c r="E2" s="10">
         <f>180-_xlfn.NUMBERVALUE(E1)</f>
-        <v>147.25000000000011</v>
+        <v>148.24999999999989</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1507,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD549D5-098D-4E2B-9746-53141BD9296F}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,10 +1693,12 @@
       <c r="D9" s="4">
         <v>0.72916666666666663</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5">
+        <v>30</v>
+      </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0.31249999999999994</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>38</v>
@@ -1757,7 +1760,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1771,11 +1774,11 @@
         <v>0.75</v>
       </c>
       <c r="E13" s="5">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>0.3125</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>40</v>
@@ -2555,7 +2558,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>1.364583333333333</v>
+        <v>1.3229166666666667</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sub struct is returning correct int values but not door values
Using a workaround for the doors which is working. Surface function doesn't seem to do anything
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B49CCF-A637-4A05-B5AA-94D1FDA53CC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEB5411-F041-4B3F-940C-89AA3EA6D44C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33990" yWindow="570" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,12 @@
   <si>
     <t>More work on the game loop files - created a function to return the sub stats that I can call after any user action. Created a temp function to seal all the doors so I can test the movement before anything else. Successfully managing to alter the depth and return a different value but it's not the values I'm expecting - think there's a problem with data type conversion when converting into C. 
 Overall, there's a skeleton game loop created in SPARK which is allowing me to access and manipulate the sub pos and movements from Unity which seems like a decent proof of concept but there are still some bugs to work out.</t>
+  </si>
+  <si>
+    <t>Added in a reset function so that the sub can be reset within the same session if needed. Appears to be working so far (only tested on locks and depth).
+Some testing was done on the functions to make sure that nothing is executing without being explicitly called (either because of unexpected dll behaviour or poor key press code or something else) - results were positive, the existing functions are only being executed when desired (rules out the unexpected depth variable being a result of this).
+Spent a significant amount of time looking into Ada to C conversions and int storage sizes (was convinced there was a conversion issue). Later realised that the front space was not updating so looked into retrieving sub stats outwith the custom sub struct and discovered they work fine so the problem was with everything being mapped into the first attribute in the struct.
+Moved onto the door functionality - more problems with that. Solution: a workaround that returns specific csharp bools rather than the values within the sub struct itself</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>31.750000000000082</c:v>
+                  <c:v>40.750000000000085</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -388,7 +394,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>148.24999999999989</c:v>
+                  <c:v>139.24999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1476,7 +1482,7 @@
       </c>
       <c r="E1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>31.750000000000082</v>
+        <v>40.750000000000085</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1485,14 +1491,14 @@
       </c>
       <c r="B2" s="9">
         <f ca="1">B1-TODAY()</f>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="10">
         <f>180-_xlfn.NUMBERVALUE(E1)</f>
-        <v>148.24999999999989</v>
+        <v>139.24999999999989</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1508,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD549D5-098D-4E2B-9746-53141BD9296F}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,21 +1838,29 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
       <c r="B17" s="1">
         <v>43634</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E17" s="5">
+        <v>30</v>
+      </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="11"/>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -2558,7 +2572,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>1.3229166666666667</v>
+        <v>1.6979166666666667</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Torpedo safe dist functionality tested and working
Moving onto game elements for now
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD39398-0B12-4E1B-9CB3-40CD8C10E4B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2260A280-49A4-42E9-9C57-684D513348E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33990" yWindow="570" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="180HrPlan" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -171,8 +170,9 @@
 Moved onto the door functionality - more problems with that. Solution: a workaround that returns specific csharp bools rather than the values within the sub struct itself</t>
   </si>
   <si>
-    <t>Had a meeting (8am) to clarify several aspects of the program/game functionality.
-Worked on adding in the functions for firing and reloading the torpedos plus added some logic in Unity re: pre and post function call state comparison.</t>
+    <t xml:space="preserve">Had a meeting (8am) to clarify several aspects of the program/game functionality.
+Worked on adding in the functions for firing and reloading the torpedos plus added some logic in Unity re: pre and post function call state comparison.
+Safe dist functionality is working. Going to move onto game elements for a while </t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>45.75</c:v>
+                  <c:v>28.249999999999918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -399,7 +399,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>134.25</c:v>
+                  <c:v>151.75000000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="E1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>45.75</v>
+        <v>28.249999999999918</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="E2" s="10">
         <f>180-_xlfn.NUMBERVALUE(E1)</f>
-        <v>134.25</v>
+        <v>151.75000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,7 +1867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1877,13 +1877,13 @@
       <c r="C18" s="4">
         <v>0.5</v>
       </c>
-      <c r="D18" s="4">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5">
+        <v>30</v>
+      </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>0.20833333333333337</v>
+        <v>-0.52083333333333337</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>42</v>
@@ -2583,7 +2583,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>1.90625</v>
+        <v>1.1770833333333335</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sub gameobject created with animations and movement. UI labels with real time values. Temporary basic sprites added for map boundaries
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2260A280-49A4-42E9-9C57-684D513348E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4956B6-C5BD-460C-9D0D-911A177C7849}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33990" yWindow="570" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
@@ -170,9 +170,11 @@
 Moved onto the door functionality - more problems with that. Solution: a workaround that returns specific csharp bools rather than the values within the sub struct itself</t>
   </si>
   <si>
-    <t xml:space="preserve">Had a meeting (8am) to clarify several aspects of the program/game functionality.
+    <t>Had a meeting (8am) to clarify several aspects of the program/game functionality.
 Worked on adding in the functions for firing and reloading the torpedos plus added some logic in Unity re: pre and post function call state comparison.
-Safe dist functionality is working. Going to move onto game elements for a while </t>
+Safe dist functionality is working. Going to move onto game elements for a while.
+Sub idle and sub moving animations created. Sub gameobject created with script and animations. Animation change when ready to dive is working, movement animation working when moving the sub.
+Temp UI labels added to show real time depth, temp, oxy, front space, and door positions + lock states. Some basic sprites also added to show boundaries.</t>
   </si>
 </sst>
 </file>
@@ -357,7 +359,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>28.249999999999918</c:v>
+                  <c:v>50.583333333333364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -399,7 +401,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>151.75000000000011</c:v>
+                  <c:v>129.4166666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,7 +1489,7 @@
       </c>
       <c r="E1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>28.249999999999918</v>
+        <v>50.583333333333364</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1503,7 +1505,7 @@
       </c>
       <c r="E2" s="10">
         <f>180-_xlfn.NUMBERVALUE(E1)</f>
-        <v>151.75000000000011</v>
+        <v>129.4166666666666</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,7 +1522,7 @@
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,7 +1869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1877,13 +1879,15 @@
       <c r="C18" s="4">
         <v>0.5</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="4">
+        <v>0.9375</v>
+      </c>
       <c r="E18" s="5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>-0.52083333333333337</v>
+        <v>0.40972222222222221</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>42</v>
@@ -2583,7 +2587,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>1.1770833333333335</v>
+        <v>2.1076388888888888</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sub exploding animation finished and added to unity. Not working in code yet
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EEAC7B-3EB0-4E52-AF0F-6BF7671A783B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87110C10-965A-47AE-99AA-024B8A3A7C77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -183,6 +183,13 @@
     <t>Finished the UI: Design aspects finished, values update in real time, door led indicators update appropriately, torpedo tubes empty/reload appropriately, torpedo silo empties/resets appropriately.
 Pause screen added. Appears to be working fine.
 A basic template installer created and working. Doesn't have uninstall functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed the graphics for firing a torpedo + the torpedo exploding on impact. 
+Finished the animation for the submarine exploding and added it into Unity. </t>
+  </si>
+  <si>
+    <t>To work on: Game over screen (new branch on git). Get explosion animation working from code.</t>
   </si>
 </sst>
 </file>
@@ -287,7 +294,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -367,7 +388,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>66.083333333333286</c:v>
+                  <c:v>74.083333333333428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -409,7 +430,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>113.9166666666667</c:v>
+                  <c:v>105.9166666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,7 +1518,7 @@
       </c>
       <c r="E1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>66.083333333333286</v>
+        <v>74.083333333333428</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1506,14 +1527,14 @@
       </c>
       <c r="B2" s="9">
         <f ca="1">B1-TODAY()</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="10">
         <f>180-_xlfn.NUMBERVALUE(E1)</f>
-        <v>113.9166666666667</v>
+        <v>105.9166666666666</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,7 +1551,7 @@
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,21 +2080,29 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
       <c r="B28" s="1">
         <v>43645</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
+      <c r="C28" s="4">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E28" s="5">
+        <v>30</v>
+      </c>
       <c r="F28" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="11"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -2089,7 +2118,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="11"/>
+      <c r="G29" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -2609,7 +2640,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>2.7534722222222223</v>
+        <v>3.0868055555555558</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2739,13 +2770,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:H2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>AND($B2&lt;TODAY(),ISBLANK($C2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:H61">
+  <conditionalFormatting sqref="A3:H27 A29:H61 A28:B28 E28:F28 H28">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($B3&lt;TODAY(),ISBLANK($C3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:D28">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND($B28&lt;TODAY(),ISBLANK($C28))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($B3&lt;TODAY(),ISBLANK($C3))</formula>
+      <formula>AND($B28&lt;TODAY(),ISBLANK($C28))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sub-beyond-safe-zone explosion animation and code working
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87110C10-965A-47AE-99AA-024B8A3A7C77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8A6019-2393-4B7D-A9D7-96E27CFC7443}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -190,6 +190,10 @@
   </si>
   <si>
     <t>To work on: Game over screen (new branch on git). Get explosion animation working from code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub explosion working. Code works with shooting outwith the safeDist. Need to work on the explosion triggering when it goes outwith the side boundaries (if the animation needs to be changed, it will be easy to substitute into working code). 
+Biggest difficulty - testing for incorrect code when the current SPARK code is all correct. </t>
   </si>
 </sst>
 </file>
@@ -388,7 +392,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>74.083333333333428</c:v>
+                  <c:v>63.583333333333435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -430,7 +434,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>105.9166666666666</c:v>
+                  <c:v>116.4166666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,7 +1522,7 @@
       </c>
       <c r="E1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>74.083333333333428</v>
+        <v>63.583333333333435</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1527,14 +1531,14 @@
       </c>
       <c r="B2" s="9">
         <f ca="1">B1-TODAY()</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="10">
         <f>180-_xlfn.NUMBERVALUE(E1)</f>
-        <v>105.9166666666666</v>
+        <v>116.4166666666666</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1551,7 +1555,7 @@
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,21 +2126,25 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7</v>
       </c>
       <c r="B30" s="1">
         <v>43647</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4">
+        <v>0.4375</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
       <c r="F30" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="11"/>
+        <v>-0.4375</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2640,7 +2648,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>3.0868055555555558</v>
+        <v>2.6493055555555558</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Functionality updated to include emergency surface and decreasing oxygen
Oxy and temp values now turn red when critical. Untested function added for adjusting the temp within Unity.
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E8D0DE-0933-48DE-B833-187D11C45DA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790E3607-E0C5-4A8B-A116-5821DE853727}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
@@ -139,12 +139,6 @@
     <t>Bug fixing</t>
   </si>
   <si>
-    <t>Notes (to self…)</t>
-  </si>
-  <si>
-    <t>Make this doc a bit nicer…</t>
-  </si>
-  <si>
     <t>ADA crash course: http://www.cristhianny.com/others/ada_tutorial_introduction_code.html, https://www.functionx.com/ada/Lesson01.htm
 Working through Tetris demo: https://blog.adacore.com/unity-ada
 Exported demo to Unity 2018 (to see what would go wrong - Nothing, miraculously).
@@ -203,6 +197,16 @@
   <si>
     <t>Submarine implosion animation and the corresponding Unity work to trigger it when depth is too low or front space &gt; 100 or &lt; 0
 Looked into animation blending and animation fading. Decided to change explosion animation (kept old one in Unity for now).</t>
+  </si>
+  <si>
+    <t>Added SFX</t>
+  </si>
+  <si>
+    <t>Updated the game loop files with new functions. 
+Updated Unity so that the emergency surface is fully working and triggered by low oxy and temp.
+Updated Unity to reduce the oxygen steadily by 1% every 3 seconds.
+Added code to change oxy/temp values to red when critically low/high (respectively).
+Value units update</t>
   </si>
 </sst>
 </file>
@@ -291,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -310,12 +314,55 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -499,7 +546,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>87.833333333333286</c:v>
+                  <c:v>99.833333333333272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -541,7 +588,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>92.1666666666667</c:v>
+                  <c:v>80.1666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,12 +838,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$C$2</c:f>
+              <c:f>Summary!$D$2</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,9 +859,12 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$D$1</c:f>
+              <c:f>Summary!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Days to go</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -830,12 +880,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$D$2</c:f>
+              <c:f>Summary!$C$2</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2451,10 +2501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D41196E-51D8-4EC2-819A-0D5258174D72}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2478,12 +2528,13 @@
       <c r="C1" s="8">
         <v>43678</v>
       </c>
+      <c r="D1" s="14"/>
       <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>87.833333333333286</v>
+        <v>99.833333333333272</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -2492,21 +2543,23 @@
       </c>
       <c r="C2" s="9">
         <f ca="1">C1-TODAY()</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="14">
         <f ca="1">COUNT(Tracker!B2:B61)-C2</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="10">
         <f>180-_xlfn.NUMBERVALUE(F1)</f>
-        <v>92.1666666666667</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25"/>
+        <v>80.1666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="15"/>
+    </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
     </row>
@@ -2525,6 +2578,12 @@
     <row r="17" x14ac:dyDescent="0.25"/>
     <row r="18" x14ac:dyDescent="0.25"/>
     <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="23" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="25" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{166A9904-6244-4FE1-933C-B9AD569A210A}">
@@ -2540,24 +2599,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD549D5-098D-4E2B-9746-53141BD9296F}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="103.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="145.85546875" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
@@ -2579,11 +2638,8 @@
       <c r="G1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2598,11 +2654,8 @@
         <v>0</v>
       </c>
       <c r="G2" s="11"/>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2618,7 +2671,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2639,10 +2692,10 @@
         <v>0.11458333333333331</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2658,7 +2711,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2679,10 +2732,10 @@
         <v>0.27083333333333326</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2698,7 +2751,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2714,7 +2767,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2735,10 +2788,10 @@
         <v>0.29166666666666663</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2754,7 +2807,7 @@
       </c>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2770,7 +2823,7 @@
       </c>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -2791,10 +2844,10 @@
         <v>0.35416666666666663</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2815,10 +2868,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -2834,7 +2887,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -2850,7 +2903,7 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -2887,7 +2940,7 @@
         <v>0.37500000000000006</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -2911,7 +2964,7 @@
         <v>0.40972222222222221</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3013,7 +3066,7 @@
         <v>0.125</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3069,7 +3122,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3093,7 +3146,7 @@
         <v>0.33333333333333337</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3111,7 +3164,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3135,7 +3188,7 @@
         <v>0.23958333333333334</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3223,7 +3276,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3297,14 +3350,22 @@
       <c r="B40" s="1">
         <v>43657</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
+      <c r="C40" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
       <c r="F40" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="11"/>
+        <v>0.22916666666666669</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -3322,21 +3383,29 @@
       </c>
       <c r="G41" s="11"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>8</v>
       </c>
       <c r="B42" s="1">
         <v>43659</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="5"/>
+      <c r="C42" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.9375</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
       <c r="F42" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="11"/>
+        <v>0.27083333333333337</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -3648,7 +3717,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>3.6597222222222228</v>
+        <v>4.1597222222222223</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3784,39 +3853,69 @@
       <pageSetup orientation="landscape" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="A2:H2">
-    <cfRule type="expression" dxfId="6" priority="7">
+  <conditionalFormatting sqref="A2:G2">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>AND($B2&lt;TODAY(),ISBLANK($C2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:H27 A29:H29 A28:B28 E28:F28 H28 A31:H34 A30:F30 H30 A36:H61 A35:B35 E35:F35 H35">
-    <cfRule type="expression" dxfId="5" priority="6">
+  <conditionalFormatting sqref="A3:G27 A29:G29 A28:B28 E28:F28 A31:G34 A30:F30 A36:G39 A35:B35 E35:F35 A41:F41 A40:B40 F40 A43:G61 A42:B42 D42:F42">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>AND($B3&lt;TODAY(),ISBLANK($C3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:D28">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>AND($B28&lt;TODAY(),ISBLANK($C28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>AND($B28&lt;TODAY(),ISBLANK($C28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND($B30&lt;TODAY(),ISBLANK($C30))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:D35">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>AND($B35&lt;TODAY(),ISBLANK($C35))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>AND($B35&lt;TODAY(),ISBLANK($C35))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>AND($B40&lt;TODAY(),ISBLANK($C40))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:D40">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>AND($B40&lt;TODAY(),ISBLANK($C40))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>AND($B42&lt;TODAY(),ISBLANK($C42))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($B41&lt;TODAY(),ISBLANK($C41))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND($B40&lt;TODAY(),ISBLANK($C40))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($B35&lt;TODAY(),ISBLANK($C35))</formula>
+      <formula>AND($B42&lt;TODAY(),ISBLANK($C42))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Installer files updated, Unity build remove from repo, add updated installer
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcmcg\Documents\University\Year3\Tri3\ProfIntern\SparkSub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790E3607-E0C5-4A8B-A116-5821DE853727}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53886367-03B0-4640-B90F-53CC16356A2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
+    <workbookView xWindow="930" yWindow="645" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CB9FD8D5-B656-499E-98CA-EE761136C74F}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,19 @@
 Updated Unity to reduce the oxygen steadily by 1% every 3 seconds.
 Added code to change oxy/temp values to red when critically low/high (respectively).
 Value units update</t>
+  </si>
+  <si>
+    <t>Started dedicated error testing - editing, rebuilding, and testing the SPARK dll for the various conditions needing tested (a selection)
+Adding the various error catching code into Unity
+Added a warning system for things that don't logically break the system but should be flagged as issues</t>
+  </si>
+  <si>
+    <t>Continued testing. Created incorrect scenarios in Unity to test the trigger for the correct death/warning response.</t>
+  </si>
+  <si>
+    <t>More testing.
+Optimised and tidied up some code (changed the sub stat update process).
+Updated the installers.</t>
   </si>
 </sst>
 </file>
@@ -546,7 +559,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>99.833333333333272</c:v>
+                  <c:v>120.33333333333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -588,7 +601,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80.1666666666667</c:v>
+                  <c:v>59.666666666666998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -843,7 +856,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,7 +898,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2534,7 +2547,7 @@
       </c>
       <c r="F1" s="10">
         <f>_xlfn.NUMBERVALUE(Tracker!F62)*24</f>
-        <v>99.833333333333272</v>
+        <v>120.33333333333337</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -2543,18 +2556,18 @@
       </c>
       <c r="C2" s="9">
         <f ca="1">C1-TODAY()</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" s="14">
         <f ca="1">COUNT(Tracker!B2:B61)-C2</f>
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="10">
         <f>180-_xlfn.NUMBERVALUE(F1)</f>
-        <v>80.1666666666667</v>
+        <v>59.666666666666998</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -2601,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD549D5-098D-4E2B-9746-53141BD9296F}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2767,7 +2780,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -3439,21 +3452,27 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
       <c r="B45" s="1">
         <v>43662</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+      <c r="C45" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E45" s="5"/>
       <c r="F45" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="11"/>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -3478,30 +3497,46 @@
       <c r="B47" s="1">
         <v>43664</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="5"/>
+      <c r="C47" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E47" s="5">
+        <v>30</v>
+      </c>
       <c r="F47" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="11"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9</v>
       </c>
       <c r="B48" s="1">
         <v>43665</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="5"/>
+      <c r="C48" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E48" s="5">
+        <v>30</v>
+      </c>
       <c r="F48" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="11"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -3717,7 +3752,7 @@
       <c r="D62" s="3"/>
       <c r="F62" s="6">
         <f>SUM(F2:F61)</f>
-        <v>4.1597222222222223</v>
+        <v>5.0138888888888893</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3858,7 +3893,7 @@
       <formula>AND($B2&lt;TODAY(),ISBLANK($C2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:G27 A29:G29 A28:B28 E28:F28 A31:G34 A30:F30 A36:G39 A35:B35 E35:F35 A41:F41 A40:B40 F40 A43:G61 A42:B42 D42:F42">
+  <conditionalFormatting sqref="A3:G27 A29:G29 A28:B28 E28:F28 A31:G34 A30:F30 A36:G39 A35:B35 E35:F35 A41:F41 A40:B40 F40 A42:B42 D42:F42 A43:G61">
     <cfRule type="expression" dxfId="11" priority="12">
       <formula>AND($B3&lt;TODAY(),ISBLANK($C3))</formula>
     </cfRule>
@@ -3928,7 +3963,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>